<commit_message>
[FIX] New method implemented by crossover tools
</commit_message>
<xml_diff>
--- a/excel_files/case_1.xlsx
+++ b/excel_files/case_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1108361138\OneDrive\Escritorio\Carpetas del Desktop\Programacion\NEXA Projects\Python_NEXA\NEXA_COURSE_ORDERING_PROGRAM\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92343809-1176-409F-BE31-F0969F64572F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C87D3D-AA53-4520-9850-4AB4D649A29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Nombre de curso</t>
   </si>
@@ -414,7 +414,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,8 +446,8 @@
       <c r="B2">
         <v>240</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>